<commit_message>
Want to delete stor_createAns
And clac functions can be used when one Matrix *p is ans
</commit_message>
<xml_diff>
--- a/附加文件/功能说明.xlsx
+++ b/附加文件/功能说明.xlsx
@@ -1228,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>

</xml_diff>